<commit_message>
version 0.3.4 is created
</commit_message>
<xml_diff>
--- a/docs/source/_static/data/reports/IFDAT_REPORT.xlsx
+++ b/docs/source/_static/data/reports/IFDAT_REPORT.xlsx
@@ -14,9 +14,9 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CONTENTS'!$A$1:$A$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'RAS'!$A$1:$J$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'OAS'!$A$1:$M$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SHR'!$A$1:$H$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'RAS'!$A$1:$J$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'OAS'!$A$1:$M$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SHR'!$A$1:$H$6</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -635,7 +635,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -649,11 +649,11 @@
     <col width="10.4" customWidth="1" min="1" max="1"/>
     <col width="27.3" customWidth="1" min="2" max="2"/>
     <col width="27.3" customWidth="1" min="3" max="3"/>
-    <col width="11.7" customWidth="1" min="4" max="4"/>
+    <col width="32.5" customWidth="1" min="4" max="4"/>
     <col width="27.3" customWidth="1" min="5" max="5"/>
     <col width="10.4" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
-    <col width="14.3" customWidth="1" min="8" max="8"/>
+    <col width="27.3" customWidth="1" min="8" max="8"/>
     <col width="18.2" customWidth="1" min="9" max="9"/>
     <col width="20.8" customWidth="1" min="10" max="10"/>
   </cols>
@@ -786,7 +786,9 @@
       <c r="B4" s="11" t="n">
         <v>44075</v>
       </c>
-      <c r="C4" s="11" t="inlineStr"/>
+      <c r="C4" s="11" t="n">
+        <v>45545</v>
+      </c>
       <c r="D4" s="5" t="inlineStr">
         <is>
           <t>LJM1</t>
@@ -814,39 +816,277 @@
       </c>
     </row>
     <row r="5" ht="36" customHeight="1">
-      <c r="A5" s="13" t="inlineStr">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>EGRJM1</t>
+        </is>
+      </c>
+      <c r="B5" s="11" t="n">
+        <v>45545</v>
+      </c>
+      <c r="C5" s="11" t="n">
+        <v>45555</v>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>LJM1</t>
+        </is>
+      </c>
+      <c r="E5" s="12" t="n">
+        <v>36526</v>
+      </c>
+      <c r="F5" s="12" t="inlineStr"/>
+      <c r="G5" s="5" t="inlineStr"/>
+      <c r="H5" s="5" t="inlineStr">
+        <is>
+          <t>JM1 ΑΕΔΑΚ</t>
+        </is>
+      </c>
+      <c r="I5" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ3</t>
+        </is>
+      </c>
+      <c r="J5" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ3</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="36" customHeight="1">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>EGRJM1</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>45555</v>
+      </c>
+      <c r="C6" s="11" t="inlineStr"/>
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>LJM1</t>
+        </is>
+      </c>
+      <c r="E6" s="12" t="n">
+        <v>36526</v>
+      </c>
+      <c r="F6" s="12" t="inlineStr"/>
+      <c r="G6" s="5" t="inlineStr"/>
+      <c r="H6" s="5" t="inlineStr">
+        <is>
+          <t>JM1 ΑΕΔΑΚ</t>
+        </is>
+      </c>
+      <c r="I6" s="5" t="inlineStr"/>
+      <c r="J6" s="5" t="inlineStr"/>
+    </row>
+    <row r="7" ht="36" customHeight="1">
+      <c r="A7" s="13" t="inlineStr">
         <is>
           <t>EGRJ1</t>
         </is>
       </c>
-      <c r="B5" s="14" t="n">
+      <c r="B7" s="14" t="n">
         <v>37711</v>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>LJ1</t>
-        </is>
-      </c>
-      <c r="E5" s="15" t="n">
+      <c r="C7" s="14" t="n">
+        <v>37987</v>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>LJ01</t>
+        </is>
+      </c>
+      <c r="E7" s="15" t="n">
         <v>37711</v>
       </c>
-      <c r="F5" s="15" t="inlineStr"/>
-      <c r="G5" s="3" t="inlineStr"/>
-      <c r="H5" s="3" t="inlineStr">
+      <c r="F7" s="15" t="inlineStr"/>
+      <c r="G7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>J1CDRCHECK ΑΕΕΑΠ</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr"/>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>EGRJ1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8" ht="36" customHeight="1">
+      <c r="A8" s="13" t="inlineStr">
+        <is>
+          <t>EGRJ1</t>
+        </is>
+      </c>
+      <c r="B8" s="14" t="n">
+        <v>37987</v>
+      </c>
+      <c r="C8" s="14" t="n">
+        <v>40544</v>
+      </c>
+      <c r="D8" s="3" t="inlineStr">
+        <is>
+          <t>LJ01</t>
+        </is>
+      </c>
+      <c r="E8" s="15" t="n">
+        <v>37711</v>
+      </c>
+      <c r="F8" s="15" t="inlineStr"/>
+      <c r="G8" s="3" t="inlineStr"/>
+      <c r="H8" s="3" t="inlineStr">
+        <is>
+          <t>J1CDRCHK2 ΑΕΕΑΠ</t>
+        </is>
+      </c>
+      <c r="I8" s="3" t="inlineStr"/>
+      <c r="J8" s="3" t="inlineStr">
+        <is>
+          <t>EGRJ1</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="36" customHeight="1">
+      <c r="A9" s="13" t="inlineStr">
+        <is>
+          <t>EGRJ1</t>
+        </is>
+      </c>
+      <c r="B9" s="14" t="n">
+        <v>40544</v>
+      </c>
+      <c r="C9" s="14" t="inlineStr"/>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>LJ01</t>
+        </is>
+      </c>
+      <c r="E9" s="15" t="n">
+        <v>37711</v>
+      </c>
+      <c r="F9" s="15" t="inlineStr"/>
+      <c r="G9" s="3" t="inlineStr"/>
+      <c r="H9" s="3" t="inlineStr">
         <is>
           <t>J1 ΑΕΕΑΠ</t>
         </is>
       </c>
-      <c r="I5" s="3" t="inlineStr"/>
-      <c r="J5" s="3" t="inlineStr">
+      <c r="I9" s="3" t="inlineStr"/>
+      <c r="J9" s="3" t="inlineStr">
         <is>
           <t>EGRJ1</t>
         </is>
       </c>
     </row>
+    <row r="10" ht="36" customHeight="1">
+      <c r="A10" s="10" t="inlineStr">
+        <is>
+          <t>EGRJM2</t>
+        </is>
+      </c>
+      <c r="B10" s="11" t="n">
+        <v>45536</v>
+      </c>
+      <c r="C10" s="11" t="n">
+        <v>45545</v>
+      </c>
+      <c r="D10" s="5" t="inlineStr">
+        <is>
+          <t>TGR909999901, LJM_____2</t>
+        </is>
+      </c>
+      <c r="E10" s="12" t="n">
+        <v>45536</v>
+      </c>
+      <c r="F10" s="12" t="inlineStr"/>
+      <c r="G10" s="5" t="inlineStr"/>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>JOURNEY ΑΕΔΑΚ 00002</t>
+        </is>
+      </c>
+      <c r="I10" s="5" t="inlineStr"/>
+      <c r="J10" s="5" t="inlineStr"/>
+    </row>
+    <row r="11" ht="36" customHeight="1">
+      <c r="A11" s="10" t="inlineStr">
+        <is>
+          <t>EGRJM2</t>
+        </is>
+      </c>
+      <c r="B11" s="11" t="n">
+        <v>45545</v>
+      </c>
+      <c r="C11" s="11" t="n">
+        <v>45550</v>
+      </c>
+      <c r="D11" s="5" t="inlineStr">
+        <is>
+          <t>TGR909999901, LJM_____2</t>
+        </is>
+      </c>
+      <c r="E11" s="12" t="n">
+        <v>45536</v>
+      </c>
+      <c r="F11" s="12" t="inlineStr"/>
+      <c r="G11" s="5" t="inlineStr"/>
+      <c r="H11" s="5" t="inlineStr">
+        <is>
+          <t>JOURNEY ΑΕΔΑΚ 02</t>
+        </is>
+      </c>
+      <c r="I11" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ2</t>
+        </is>
+      </c>
+      <c r="J11" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ2</t>
+        </is>
+      </c>
+    </row>
+    <row r="12" ht="36" customHeight="1">
+      <c r="A12" s="10" t="inlineStr">
+        <is>
+          <t>EGRJM2</t>
+        </is>
+      </c>
+      <c r="B12" s="11" t="n">
+        <v>45550</v>
+      </c>
+      <c r="C12" s="11" t="inlineStr"/>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>TGR909999901, LJM_____2</t>
+        </is>
+      </c>
+      <c r="E12" s="12" t="n">
+        <v>45536</v>
+      </c>
+      <c r="F12" s="12" t="inlineStr"/>
+      <c r="G12" s="5" t="inlineStr"/>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>JOURNEY ΑΕΔΑΚ 02</t>
+        </is>
+      </c>
+      <c r="I12" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ2, EGRJ4</t>
+        </is>
+      </c>
+      <c r="J12" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ2, EGRJ4</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J5"/>
+  <autoFilter ref="A1:J12"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -857,7 +1097,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -873,7 +1113,7 @@
     <col width="27.3" customWidth="1" min="3" max="3"/>
     <col width="11.7" customWidth="1" min="4" max="4"/>
     <col width="27.3" customWidth="1" min="5" max="5"/>
-    <col width="10.4" customWidth="1" min="6" max="6"/>
+    <col width="27.3" customWidth="1" min="6" max="6"/>
     <col width="13" customWidth="1" min="7" max="7"/>
     <col width="50" customWidth="1" min="8" max="8"/>
     <col width="24.7" customWidth="1" min="9" max="9"/>
@@ -958,10 +1198,12 @@
       <c r="B2" s="11" t="n">
         <v>37711</v>
       </c>
-      <c r="C2" s="11" t="inlineStr"/>
+      <c r="C2" s="11" t="n">
+        <v>37987</v>
+      </c>
       <c r="D2" s="5" t="inlineStr">
         <is>
-          <t>LJ1</t>
+          <t>LJ01</t>
         </is>
       </c>
       <c r="E2" s="12" t="n">
@@ -971,7 +1213,7 @@
       <c r="G2" s="5" t="inlineStr"/>
       <c r="H2" s="5" t="inlineStr">
         <is>
-          <t>J1 ΑΕΕΑΠ</t>
+          <t>J1CDRCHECK ΑΕΕΑΠ</t>
         </is>
       </c>
       <c r="I2" s="5" t="inlineStr">
@@ -993,150 +1235,338 @@
       <c r="M2" s="5" t="inlineStr"/>
     </row>
     <row r="3" ht="36" customHeight="1">
-      <c r="A3" s="13" t="inlineStr">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>EGRJ1</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>37987</v>
+      </c>
+      <c r="C3" s="11" t="n">
+        <v>40544</v>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>LJ01</t>
+        </is>
+      </c>
+      <c r="E3" s="12" t="n">
+        <v>37711</v>
+      </c>
+      <c r="F3" s="12" t="inlineStr"/>
+      <c r="G3" s="5" t="inlineStr"/>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>J1CDRCHK2 ΑΕΕΑΠ</t>
+        </is>
+      </c>
+      <c r="I3" s="5" t="inlineStr">
+        <is>
+          <t>RES</t>
+        </is>
+      </c>
+      <c r="J3" s="5" t="inlineStr"/>
+      <c r="K3" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ1</t>
+        </is>
+      </c>
+      <c r="L3" s="5" t="inlineStr">
+        <is>
+          <t>IGRS487003126</t>
+        </is>
+      </c>
+      <c r="M3" s="5" t="inlineStr"/>
+    </row>
+    <row r="4" ht="36" customHeight="1">
+      <c r="A4" s="10" t="inlineStr">
+        <is>
+          <t>EGRJ1</t>
+        </is>
+      </c>
+      <c r="B4" s="11" t="n">
+        <v>40544</v>
+      </c>
+      <c r="C4" s="11" t="inlineStr"/>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>LJ01</t>
+        </is>
+      </c>
+      <c r="E4" s="12" t="n">
+        <v>37711</v>
+      </c>
+      <c r="F4" s="12" t="inlineStr"/>
+      <c r="G4" s="5" t="inlineStr"/>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>J1 ΑΕΕΑΠ</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t>RES</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr"/>
+      <c r="K4" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ1</t>
+        </is>
+      </c>
+      <c r="L4" s="5" t="inlineStr">
+        <is>
+          <t>IGRS487003126</t>
+        </is>
+      </c>
+      <c r="M4" s="5" t="inlineStr"/>
+    </row>
+    <row r="5" ht="36" customHeight="1">
+      <c r="A5" s="13" t="inlineStr">
         <is>
           <t>EGRJ2</t>
         </is>
       </c>
-      <c r="B3" s="14" t="n">
+      <c r="B5" s="14" t="n">
         <v>39321</v>
       </c>
-      <c r="C3" s="14" t="n">
+      <c r="C5" s="14" t="n">
         <v>43704</v>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>LJ2</t>
         </is>
       </c>
-      <c r="E3" s="15" t="n">
+      <c r="E5" s="15" t="n">
         <v>39321</v>
       </c>
-      <c r="F3" s="15" t="inlineStr"/>
-      <c r="G3" s="3" t="inlineStr"/>
-      <c r="H3" s="3" t="inlineStr">
+      <c r="F5" s="15" t="inlineStr"/>
+      <c r="G5" s="3" t="inlineStr"/>
+      <c r="H5" s="3" t="inlineStr">
         <is>
           <t>JM1 smart cash ομολογιακό</t>
         </is>
       </c>
-      <c r="I3" s="3" t="inlineStr">
+      <c r="I5" s="3" t="inlineStr">
         <is>
           <t>BON</t>
         </is>
       </c>
-      <c r="J3" s="3" t="inlineStr">
+      <c r="J5" s="3" t="inlineStr">
         <is>
           <t>EGRJM1</t>
         </is>
       </c>
-      <c r="K3" s="3" t="inlineStr">
+      <c r="K5" s="3" t="inlineStr">
         <is>
           <t>EGRJM1</t>
         </is>
       </c>
-      <c r="L3" s="3" t="inlineStr">
+      <c r="L5" s="3" t="inlineStr">
         <is>
           <t>IGRF500121049</t>
         </is>
       </c>
-      <c r="M3" s="3" t="inlineStr"/>
-    </row>
-    <row r="4" ht="36" customHeight="1">
-      <c r="A4" s="13" t="inlineStr">
+      <c r="M5" s="3" t="inlineStr"/>
+    </row>
+    <row r="6" ht="36" customHeight="1">
+      <c r="A6" s="13" t="inlineStr">
         <is>
           <t>EGRJ2</t>
         </is>
       </c>
-      <c r="B4" s="14" t="n">
+      <c r="B6" s="14" t="n">
         <v>43704</v>
       </c>
-      <c r="C4" s="14" t="inlineStr"/>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="C6" s="14" t="n">
+        <v>45545</v>
+      </c>
+      <c r="D6" s="3" t="inlineStr">
         <is>
           <t>LJ2</t>
         </is>
       </c>
-      <c r="E4" s="15" t="n">
+      <c r="E6" s="15" t="n">
         <v>39321</v>
       </c>
-      <c r="F4" s="15" t="inlineStr"/>
-      <c r="G4" s="3" t="inlineStr"/>
-      <c r="H4" s="3" t="inlineStr">
+      <c r="F6" s="15" t="inlineStr"/>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr">
         <is>
           <t>JM1 smart cash ομολογιακό</t>
         </is>
       </c>
-      <c r="I4" s="3" t="inlineStr">
+      <c r="I6" s="3" t="inlineStr">
         <is>
           <t>BON</t>
         </is>
       </c>
-      <c r="J4" s="3" t="inlineStr">
+      <c r="J6" s="3" t="inlineStr">
         <is>
           <t>EGRJM1</t>
         </is>
       </c>
-      <c r="K4" s="3" t="inlineStr">
+      <c r="K6" s="3" t="inlineStr">
         <is>
           <t>EGRJM1</t>
         </is>
       </c>
-      <c r="L4" s="3" t="inlineStr">
+      <c r="L6" s="3" t="inlineStr">
         <is>
           <t>IGRF500121049, IGRF710121049</t>
         </is>
       </c>
-      <c r="M4" s="3" t="inlineStr"/>
-    </row>
-    <row r="5" ht="36" customHeight="1">
-      <c r="A5" s="10" t="inlineStr">
+      <c r="M6" s="3" t="inlineStr"/>
+    </row>
+    <row r="7" ht="36" customHeight="1">
+      <c r="A7" s="13" t="inlineStr">
+        <is>
+          <t>EGRJ2</t>
+        </is>
+      </c>
+      <c r="B7" s="14" t="n">
+        <v>45545</v>
+      </c>
+      <c r="C7" s="14" t="inlineStr"/>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>LJ2</t>
+        </is>
+      </c>
+      <c r="E7" s="15" t="n">
+        <v>39321</v>
+      </c>
+      <c r="F7" s="15" t="inlineStr"/>
+      <c r="G7" s="3" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>JM1 smart cash ομολογιακό</t>
+        </is>
+      </c>
+      <c r="I7" s="3" t="inlineStr">
+        <is>
+          <t>BON</t>
+        </is>
+      </c>
+      <c r="J7" s="3" t="inlineStr">
+        <is>
+          <t>EGRJM2</t>
+        </is>
+      </c>
+      <c r="K7" s="3" t="inlineStr">
+        <is>
+          <t>EGRJM2</t>
+        </is>
+      </c>
+      <c r="L7" s="3" t="inlineStr">
+        <is>
+          <t>IGRF500121049, IGRF710121049</t>
+        </is>
+      </c>
+      <c r="M7" s="3" t="inlineStr"/>
+    </row>
+    <row r="8" ht="36" customHeight="1">
+      <c r="A8" s="10" t="inlineStr">
         <is>
           <t>EGRJ3</t>
         </is>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B8" s="11" t="n">
         <v>44075</v>
       </c>
-      <c r="C5" s="11" t="inlineStr"/>
-      <c r="D5" s="5" t="inlineStr">
+      <c r="C8" s="11" t="n">
+        <v>45555</v>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
         <is>
           <t>LJ3</t>
         </is>
       </c>
-      <c r="E5" s="12" t="n">
+      <c r="E8" s="12" t="n">
         <v>44075</v>
       </c>
-      <c r="F5" s="12" t="inlineStr"/>
-      <c r="G5" s="5" t="inlineStr"/>
-      <c r="H5" s="5" t="inlineStr">
+      <c r="F8" s="12" t="n">
+        <v>45555</v>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>EGRJ2</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
         <is>
           <t>JM1 Βραχυπρόθεσμο Αμοιβαίο Κεφάλαιο Χρηματαγοράς Κυμαινόμενης Καθαρής Αξίας Ενεργητικού</t>
         </is>
       </c>
-      <c r="I5" s="5" t="inlineStr">
+      <c r="I8" s="5" t="inlineStr">
         <is>
           <t>MMF</t>
         </is>
       </c>
-      <c r="J5" s="5" t="inlineStr">
+      <c r="J8" s="5" t="inlineStr">
         <is>
           <t>EGRJM1</t>
         </is>
       </c>
-      <c r="K5" s="5" t="inlineStr">
+      <c r="K8" s="5" t="inlineStr">
         <is>
           <t>EGRJM1</t>
         </is>
       </c>
-      <c r="L5" s="5" t="inlineStr">
+      <c r="L8" s="5" t="inlineStr">
         <is>
           <t>IGRF717124049</t>
         </is>
       </c>
-      <c r="M5" s="5" t="inlineStr"/>
+      <c r="M8" s="5" t="inlineStr"/>
+    </row>
+    <row r="9" ht="36" customHeight="1">
+      <c r="A9" s="13" t="inlineStr">
+        <is>
+          <t>EGRJ4</t>
+        </is>
+      </c>
+      <c r="B9" s="14" t="n">
+        <v>45550</v>
+      </c>
+      <c r="C9" s="14" t="inlineStr"/>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>LJ0004</t>
+        </is>
+      </c>
+      <c r="E9" s="15" t="n">
+        <v>45550</v>
+      </c>
+      <c r="F9" s="15" t="inlineStr"/>
+      <c r="G9" s="3" t="inlineStr"/>
+      <c r="H9" s="3" t="inlineStr">
+        <is>
+          <t>Συνθετο Journey 4</t>
+        </is>
+      </c>
+      <c r="I9" s="3" t="inlineStr">
+        <is>
+          <t>OTH</t>
+        </is>
+      </c>
+      <c r="J9" s="3" t="inlineStr">
+        <is>
+          <t>EGRJM2</t>
+        </is>
+      </c>
+      <c r="K9" s="3" t="inlineStr">
+        <is>
+          <t>EGRJM2</t>
+        </is>
+      </c>
+      <c r="L9" s="3" t="inlineStr"/>
+      <c r="M9" s="3" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M5"/>
+  <autoFilter ref="A1:M9"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1147,7 +1577,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -1160,7 +1590,7 @@
   <cols>
     <col width="19.5" customWidth="1" min="1" max="1"/>
     <col width="27.3" customWidth="1" min="2" max="2"/>
-    <col width="9.1" customWidth="1" min="3" max="3"/>
+    <col width="27.3" customWidth="1" min="3" max="3"/>
     <col width="11.7" customWidth="1" min="4" max="4"/>
     <col width="27.3" customWidth="1" min="5" max="5"/>
     <col width="10.4" customWidth="1" min="6" max="6"/>
@@ -1284,7 +1714,9 @@
       <c r="B5" s="14" t="n">
         <v>44075</v>
       </c>
-      <c r="C5" s="14" t="inlineStr"/>
+      <c r="C5" s="14" t="n">
+        <v>45555</v>
+      </c>
       <c r="D5" s="3" t="inlineStr"/>
       <c r="E5" s="15" t="n">
         <v>44075</v>
@@ -1297,8 +1729,26 @@
         </is>
       </c>
     </row>
+    <row r="6" ht="36" customHeight="1">
+      <c r="A6" s="13" t="inlineStr">
+        <is>
+          <t>IGRF717124049</t>
+        </is>
+      </c>
+      <c r="B6" s="14" t="n">
+        <v>45555</v>
+      </c>
+      <c r="C6" s="14" t="inlineStr"/>
+      <c r="D6" s="3" t="inlineStr"/>
+      <c r="E6" s="15" t="n">
+        <v>44075</v>
+      </c>
+      <c r="F6" s="15" t="inlineStr"/>
+      <c r="G6" s="3" t="inlineStr"/>
+      <c r="H6" s="3" t="inlineStr"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H5"/>
+  <autoFilter ref="A1:H6"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Datamodel, regex and IFDAT docs update
</commit_message>
<xml_diff>
--- a/docs/source/_static/data/reports/IFDAT_REPORT.xlsx
+++ b/docs/source/_static/data/reports/IFDAT_REPORT.xlsx
@@ -9,14 +9,16 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CONTENTS" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RAS" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OAS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SHR" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="USR" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="OAS" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SHR" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CONTENTS'!$A$1:$A$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'RAS'!$A$1:$J$12</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'OAS'!$A$1:$M$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'SHR'!$A$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'CONTENTS'!$A$1:$A$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'RAS'!$A$1:$K$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'USR'!$A$1:$H$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'OAS'!$A$1:$M$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'SHR'!$A$1:$H$6</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -566,7 +568,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -603,28 +605,39 @@
     </row>
     <row r="3" ht="25" customHeight="1">
       <c r="A3" s="4">
+        <f>HYPERLINK("#USR!A1", "USR")</f>
+        <v/>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Reporting Persons</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="25" customHeight="1">
+      <c r="A4" s="2">
         <f>HYPERLINK("#OAS!A1", "OAS")</f>
         <v/>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Observed Agents</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="25" customHeight="1">
-      <c r="A4" s="2">
+    <row r="5" ht="25" customHeight="1">
+      <c r="A5" s="4">
         <f>HYPERLINK("#SHR!A1", "SHR")</f>
         <v/>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B5" s="5" t="inlineStr">
         <is>
           <t>Shares/fund units/fund classes issued by Observed Agents</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A4"/>
+  <autoFilter ref="A1:A5"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -635,7 +648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -656,6 +669,7 @@
     <col width="27.3" customWidth="1" min="8" max="8"/>
     <col width="18.2" customWidth="1" min="9" max="9"/>
     <col width="20.8" customWidth="1" min="10" max="10"/>
+    <col width="15.6" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="42" customHeight="1">
@@ -708,6 +722,11 @@
           <t>IFDAT_RPRTR_OF</t>
         </is>
       </c>
+      <c r="K1" s="8" t="inlineStr">
+        <is>
+          <t>IFDAT_USRS</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="36" customHeight="1">
       <c r="A2" s="10" t="inlineStr">
@@ -738,6 +757,11 @@
       </c>
       <c r="I2" s="5" t="inlineStr"/>
       <c r="J2" s="5" t="inlineStr"/>
+      <c r="K2" s="5" t="inlineStr">
+        <is>
+          <t>juser</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="36" customHeight="1">
       <c r="A3" s="10" t="inlineStr">
@@ -776,6 +800,11 @@
           <t>EGRJ2</t>
         </is>
       </c>
+      <c r="K3" s="5" t="inlineStr">
+        <is>
+          <t>juser</t>
+        </is>
+      </c>
     </row>
     <row r="4" ht="36" customHeight="1">
       <c r="A4" s="10" t="inlineStr">
@@ -814,6 +843,11 @@
           <t>EGRJ2, EGRJ3</t>
         </is>
       </c>
+      <c r="K4" s="5" t="inlineStr">
+        <is>
+          <t>juser</t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="36" customHeight="1">
       <c r="A5" s="10" t="inlineStr">
@@ -852,6 +886,11 @@
           <t>EGRJ3</t>
         </is>
       </c>
+      <c r="K5" s="5" t="inlineStr">
+        <is>
+          <t>juser</t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="36" customHeight="1">
       <c r="A6" s="10" t="inlineStr">
@@ -880,6 +919,11 @@
       </c>
       <c r="I6" s="5" t="inlineStr"/>
       <c r="J6" s="5" t="inlineStr"/>
+      <c r="K6" s="5" t="inlineStr">
+        <is>
+          <t>juser</t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="36" customHeight="1">
       <c r="A7" s="13" t="inlineStr">
@@ -914,6 +958,7 @@
           <t>EGRJ1</t>
         </is>
       </c>
+      <c r="K7" s="3" t="inlineStr"/>
     </row>
     <row r="8" ht="36" customHeight="1">
       <c r="A8" s="13" t="inlineStr">
@@ -948,6 +993,7 @@
           <t>EGRJ1</t>
         </is>
       </c>
+      <c r="K8" s="3" t="inlineStr"/>
     </row>
     <row r="9" ht="36" customHeight="1">
       <c r="A9" s="13" t="inlineStr">
@@ -980,6 +1026,7 @@
           <t>EGRJ1</t>
         </is>
       </c>
+      <c r="K9" s="3" t="inlineStr"/>
     </row>
     <row r="10" ht="36" customHeight="1">
       <c r="A10" s="10" t="inlineStr">
@@ -1010,6 +1057,7 @@
       </c>
       <c r="I10" s="5" t="inlineStr"/>
       <c r="J10" s="5" t="inlineStr"/>
+      <c r="K10" s="5" t="inlineStr"/>
     </row>
     <row r="11" ht="36" customHeight="1">
       <c r="A11" s="10" t="inlineStr">
@@ -1048,6 +1096,7 @@
           <t>EGRJ2</t>
         </is>
       </c>
+      <c r="K11" s="5" t="inlineStr"/>
     </row>
     <row r="12" ht="36" customHeight="1">
       <c r="A12" s="10" t="inlineStr">
@@ -1084,14 +1133,159 @@
           <t>EGRJ2, EGRJ4</t>
         </is>
       </c>
+      <c r="K12" s="5" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J12"/>
+  <autoFilter ref="A1:K12"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.1" customWidth="1" min="1" max="1"/>
+    <col width="27.3" customWidth="1" min="2" max="2"/>
+    <col width="27.3" customWidth="1" min="3" max="3"/>
+    <col width="11.7" customWidth="1" min="4" max="4"/>
+    <col width="11.7" customWidth="1" min="5" max="5"/>
+    <col width="15.6" customWidth="1" min="6" max="6"/>
+    <col width="24.7" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="42" customHeight="1">
+      <c r="A1" s="6">
+        <f>HYPERLINK("#CONTENTS!A1", "ID")</f>
+        <v/>
+      </c>
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>VLD_FRM</t>
+        </is>
+      </c>
+      <c r="C1" s="7" t="inlineStr">
+        <is>
+          <t>VLD_T</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>FRST</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>LST</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>PHN</t>
+        </is>
+      </c>
+      <c r="G1" s="8" t="inlineStr">
+        <is>
+          <t>EMAIL</t>
+        </is>
+      </c>
+      <c r="H1" s="8" t="inlineStr">
+        <is>
+          <t>IFDAT_RL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="36" customHeight="1">
+      <c r="A2" s="10" t="inlineStr">
+        <is>
+          <t>juser</t>
+        </is>
+      </c>
+      <c r="B2" s="11" t="n">
+        <v>-81081</v>
+      </c>
+      <c r="C2" s="11" t="n">
+        <v>36526</v>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>Journer</t>
+        </is>
+      </c>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>Tripper</t>
+        </is>
+      </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>2106799999</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>juser@journey.org</t>
+        </is>
+      </c>
+      <c r="H2" s="5" t="inlineStr"/>
+    </row>
+    <row r="3" ht="36" customHeight="1">
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>juser</t>
+        </is>
+      </c>
+      <c r="B3" s="11" t="n">
+        <v>36526</v>
+      </c>
+      <c r="C3" s="11" t="inlineStr"/>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>Journer</t>
+        </is>
+      </c>
+      <c r="E3" s="5" t="inlineStr">
+        <is>
+          <t>Tripper</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>2106799999</t>
+        </is>
+      </c>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>juser@journey.org</t>
+        </is>
+      </c>
+      <c r="H3" s="5" t="inlineStr">
+        <is>
+          <t>EGRJM1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1571,7 +1765,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>